<commit_message>
Fixed example 3 for v2
</commit_message>
<xml_diff>
--- a/deployable examples/windows_planning_deployment_3_v2/src/walkthrough_policy_3.xlsx
+++ b/deployable examples/windows_planning_deployment_3_v2/src/walkthrough_policy_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint-df.com/personal/joshbregman_microsoft_com/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{15C5DB41-B4BD-44F2-9398-E37525A0D05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80CD4C39-D356-44A6-B79F-55C7E2F38A8D}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{15C5DB41-B4BD-44F2-9398-E37525A0D05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62A1F699-4992-4E47-B2C3-1C0121A76849}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="16380" windowHeight="10260" firstSheet="3" activeTab="3" xr2:uid="{F17E21AF-5E05-4ECF-8E29-50A77CA88224}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="16380" windowHeight="10260" activeTab="5" xr2:uid="{F17E21AF-5E05-4ECF-8E29-50A77CA88224}"/>
   </bookViews>
   <sheets>
     <sheet name="Allowed Full Access USBs" sheetId="15" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>PrimaryId</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Deny other access</t>
   </si>
   <si>
-    <t>Audit deny  and block</t>
-  </si>
-  <si>
     <t>Allow</t>
   </si>
   <si>
@@ -178,16 +175,16 @@
     <t>Allowed RO USBs, Allowed Full Access USBs</t>
   </si>
   <si>
-    <t>Grant full access to allowed full access USBs</t>
-  </si>
-  <si>
     <t>Grant RO access to allowed RO access USBs</t>
   </si>
   <si>
-    <t>allow full access</t>
-  </si>
-  <si>
     <t>allow RO access</t>
+  </si>
+  <si>
+    <t>Audit denied other access and notify only</t>
+  </si>
+  <si>
+    <t>Deny other access, Audit denied other access and notify only</t>
   </si>
 </sst>
 </file>
@@ -623,12 +620,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -648,12 +645,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -663,10 +660,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D8DADB-7CF6-48C8-A3AB-15DCC09744A3}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -705,47 +702,33 @@
     </row>
     <row r="2" spans="1:9" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -759,7 +742,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -780,7 +763,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -791,7 +774,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -802,7 +785,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -820,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409B0504-EC05-4B1B-97F5-884FF44238AD}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -863,7 +846,7 @@
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>21</v>
@@ -874,16 +857,16 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -894,10 +877,10 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -908,10 +891,10 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -922,13 +905,13 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -936,36 +919,36 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -973,19 +956,19 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -993,19 +976,19 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9">
         <v>1</v>

</xml_diff>

<commit_message>
Updated example with sending audit record
</commit_message>
<xml_diff>
--- a/deployable examples/windows_planning_deployment_3_v2/src/walkthrough_policy_3.xlsx
+++ b/deployable examples/windows_planning_deployment_3_v2/src/walkthrough_policy_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint-df.com/personal/joshbregman_microsoft_com/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{15C5DB41-B4BD-44F2-9398-E37525A0D05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62A1F699-4992-4E47-B2C3-1C0121A76849}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{15C5DB41-B4BD-44F2-9398-E37525A0D05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{868751C4-F6A0-419F-93D4-87396E1D36B6}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="16380" windowHeight="10260" activeTab="5" xr2:uid="{F17E21AF-5E05-4ECF-8E29-50A77CA88224}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="16380" windowHeight="10260" firstSheet="2" activeTab="3" xr2:uid="{F17E21AF-5E05-4ECF-8E29-50A77CA88224}"/>
   </bookViews>
   <sheets>
     <sheet name="Allowed Full Access USBs" sheetId="15" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t>PrimaryId</t>
   </si>
@@ -184,7 +184,10 @@
     <t>Audit denied other access and notify only</t>
   </si>
   <si>
-    <t>Deny other access, Audit denied other access and notify only</t>
+    <t>Audit denied other access and notify and send</t>
+  </si>
+  <si>
+    <t>Deny other access, Audit denied other access and notify and send</t>
   </si>
 </sst>
 </file>
@@ -662,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D8DADB-7CF6-48C8-A3AB-15DCC09744A3}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -728,7 +731,7 @@
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -801,10 +804,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409B0504-EC05-4B1B-97F5-884FF44238AD}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -936,13 +939,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
@@ -951,15 +951,15 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
@@ -971,12 +971,12 @@
         <v>28</v>
       </c>
       <c r="J8">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
@@ -991,6 +991,26 @@
         <v>28</v>
       </c>
       <c r="J9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10">
         <v>1</v>
       </c>
     </row>

</xml_diff>